<commit_message>
Email list data changes
</commit_message>
<xml_diff>
--- a/AutomationTesting/src/main/java/com/engexcellence/qa/testdata/Email_List_Test_data.xlsx
+++ b/AutomationTesting/src/main/java/com/engexcellence/qa/testdata/Email_List_Test_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omgoyal\Selenium_Workspace\AutomationTesting\src\main\java\com\engexcellence\qa\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Workspace\Automation_Testing\AutomationTesting\src\main\java\com\engexcellence\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CDC69C-BEBC-4994-9858-0B97BF29FFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52207A9-07B8-4B18-85F4-A4D56B819FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3FE68D40-7A67-436C-97BD-CA94B2991C58}"/>
   </bookViews>
@@ -47,13 +47,13 @@
     <t>osgoyal@gmail.com</t>
   </si>
   <si>
-    <t>5$August$92</t>
-  </si>
-  <si>
     <t>toshobhna.gupta@gmail.com</t>
   </si>
   <si>
     <t>!@#$%^&amp;*</t>
+  </si>
+  <si>
+    <t>$#$%$$%^^</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,15 +441,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>